<commit_message>
add data of 12 to calculation_estimate.xlsx
</commit_message>
<xml_diff>
--- a/calculation_estimate.xlsx
+++ b/calculation_estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkoba\Documents\kosuke\C++_program\Knot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59C544B-35CE-4F96-BD94-324DB67B7205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59B362F-6C2B-4533-8730-8E2EA122F3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95B1DAC3-A618-4BEB-AC30-76479A61DF31}"/>
   </bookViews>
@@ -247,10 +247,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2.7725887222397811</c:v>
                 </c:pt>
@@ -280,6 +280,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>17.480673383060889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.090111377414996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,49 +339,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.9045357080890488</c:v>
+                  <c:v>2.9114321376519063</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5281506567010688</c:v>
+                  <c:v>4.5327482764096416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1517656053130887</c:v>
+                  <c:v>6.154064415167376</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.7753805539251086</c:v>
+                  <c:v>7.7753805539251113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3989955025371277</c:v>
+                  <c:v>9.3966966926828466</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.022610451149149</c:v>
+                  <c:v>11.018012831440581</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.646225399761169</c:v>
+                  <c:v>12.639328970198317</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.269840348373188</c:v>
+                  <c:v>14.260645108956052</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.893455296985207</c:v>
+                  <c:v>15.881961247713786</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.517070245597225</c:v>
+                  <c:v>17.503277386471524</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.140685194209247</c:v>
+                  <c:v>19.124593525229258</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.76430014282127</c:v>
+                  <c:v>20.745909663986993</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.387915091433285</c:v>
+                  <c:v>22.367225802744727</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.011530040045308</c:v>
+                  <c:v>23.988541941502461</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.635144988657331</c:v>
+                  <c:v>25.609858080260196</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,7 +585,582 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>steps</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>steps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="12"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$2:$C$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2496</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>312496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1562496</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7812496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39062496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>195312496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-46A9-46DD-A0EA-B65B9EAB8E55}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>est steps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="12"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$F$2:$F$16</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>18.383106863468594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.013837872240188</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>470.62632557046254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2381.2493214631477</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12048.514974370537</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60962.416568137407</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>308454.29845359683</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1560700.1754623419</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7896745.3198082717</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39955519.725267515</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>202164751.66189054</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1022902144.5732234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-46A9-46DD-A0EA-B65B9EAB8E55}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="266582720"/>
+        <c:axId val="266578880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="266582720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266578880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="266578880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="266582720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1138,20 +1716,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>214312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1171,6 +2252,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>233362</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4008A9-F349-0A8A-BA63-DF96AF4AD538}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1499,7 +2616,7 @@
   <dimension ref="B1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1532,18 +2649,18 @@
       </c>
       <c r="E2">
         <f>B2*$H$2+$I$2</f>
-        <v>2.9045357080890488</v>
+        <v>2.9114321376519063</v>
       </c>
       <c r="F2">
         <f>EXP(E2)</f>
-        <v>18.256765215716953</v>
+        <v>18.383106863468594</v>
       </c>
       <c r="H2" cm="1">
-        <f t="array" ref="H2:I2">LINEST(D2:D11,B2:B11)</f>
-        <v>1.6236149486120199</v>
+        <f t="array" ref="H2:I2">LINEST(D2:D12,B2:B12)</f>
+        <v>1.6213161387577351</v>
       </c>
       <c r="I2">
-        <v>1.2809207594770289</v>
+        <v>1.2901159988941711</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.4">
@@ -1560,11 +2677,11 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E16" si="1">B3*$H$2+$I$2</f>
-        <v>4.5281506567010688</v>
+        <v>4.5327482764096416</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F16" si="2">EXP(E3)</f>
-        <v>92.587177181435578</v>
+        <v>93.013837872240188</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.4">
@@ -1581,11 +2698,11 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>6.1517656053130887</v>
+        <v>6.154064415167376</v>
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>469.54568770193293</v>
+        <v>470.62632557046254</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
@@ -1602,11 +2719,11 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>7.7753805539251086</v>
+        <v>7.7753805539251113</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>2381.2493214631413</v>
+        <v>2381.2493214631477</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
@@ -1623,11 +2740,11 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>9.3989955025371277</v>
+        <v>9.3966966926828466</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>12076.244079081389</v>
+        <v>12048.514974370537</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
@@ -1644,11 +2761,11 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>11.022610451149149</v>
+        <v>11.018012831440581</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>61243.343879649226</v>
+        <v>60962.416568137407</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.4">
@@ -1665,11 +2782,11 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>12.646225399761169</v>
+        <v>12.639328970198317</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>310588.88384494121</v>
+        <v>308454.29845359683</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.4">
@@ -1686,11 +2803,11 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>14.269840348373188</v>
+        <v>14.260645108956052</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>1575117.3704298839</v>
+        <v>1560700.1754623419</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
@@ -1707,11 +2824,11 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>15.893455296985207</v>
+        <v>15.881961247713786</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>7988034.5359319653</v>
+        <v>7896745.3198082717</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
@@ -1728,11 +2845,11 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>17.517070245597225</v>
+        <v>17.503277386471524</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>40510438.742623292</v>
+        <v>39955519.725267515</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
@@ -1740,17 +2857,20 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="D12" t="e">
+      <c r="C12">
+        <v>195312496</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>19.090111377414996</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>19.140685194209247</v>
+        <v>19.124593525229258</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>205444235.34197655</v>
+        <v>202164751.66189054</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
@@ -1764,11 +2884,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>20.76430014282127</v>
+        <v>20.745909663986993</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>1041887847.806515</v>
+        <v>1022902144.5732234</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
@@ -1782,11 +2902,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>22.387915091433285</v>
+        <v>22.367225802744727</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>5283819648.674696</v>
+        <v>5175624280.5492983</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
@@ -1800,11 +2920,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>24.011530040045308</v>
+        <v>23.988541941502461</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>26796310311.61203</v>
+        <v>26187340436.740974</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
@@ -1818,11 +2938,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>25.635144988657331</v>
+        <v>25.609858080260196</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>135894541081.90593</v>
+        <v>132501271726.19771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>